<commit_message>
dia 2020-06-20 tem -148 casos
</commit_message>
<xml_diff>
--- a/owid-covid-data.xlsx
+++ b/owid-covid-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igorm\Desktop\FGV\4º Semestre\03 - Modelagem de Fenômenos Biológicos\MM4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B0F7E5-54A1-4481-980B-FC691DD6A01B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE640D3-5069-4322-84E1-3A14C4080DBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1432,9 +1432,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO304"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F174" sqref="F174"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>